<commit_message>
updated waybill bulk upload
</commit_message>
<xml_diff>
--- a/public/templates/customers/shipments-bulk.xlsx
+++ b/public/templates/customers/shipments-bulk.xlsx
@@ -27,17 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Remarks</t>
   </si>
   <si>
-    <t>Number Of Items</t>
-  </si>
-  <si>
-    <t>Type Of Items</t>
-  </si>
-  <si>
     <t>Length</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>Package Type</t>
   </si>
   <si>
-    <t>From</t>
-  </si>
-  <si>
     <t>Contact Person</t>
   </si>
   <si>
@@ -93,6 +84,18 @@
   </si>
   <si>
     <t>Delivery Address</t>
+  </si>
+  <si>
+    <t>Shipper Contact Number</t>
+  </si>
+  <si>
+    <t>Shipper Address</t>
+  </si>
+  <si>
+    <t>Shipper Name</t>
+  </si>
+  <si>
+    <t>Address Type</t>
   </si>
 </sst>
 </file>
@@ -417,95 +420,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="22.5" customWidth="1"/>
-    <col min="18" max="18" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28" customWidth="1"/>
-    <col min="20" max="20" width="30.83203125" customWidth="1"/>
-    <col min="21" max="21" width="16.5" customWidth="1"/>
-    <col min="22" max="22" width="25.83203125" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" customWidth="1"/>
-    <col min="27" max="27" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="25" customWidth="1"/>
+    <col min="4" max="7" width="27.5" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" customWidth="1"/>
+    <col min="9" max="18" width="22.5" customWidth="1"/>
+    <col min="19" max="19" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28" customWidth="1"/>
+    <col min="21" max="21" width="30.83203125" customWidth="1"/>
+    <col min="22" max="22" width="16.5" customWidth="1"/>
+    <col min="23" max="23" width="25.83203125" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" customWidth="1"/>
+    <col min="28" max="28" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>